<commit_message>
updated creation of Excel files from pcap to include "0x" prefix to codes for downstream lookup
</commit_message>
<xml_diff>
--- a/data/EMSSecurityAccessFailure.xlsx
+++ b/data/EMSSecurityAccessFailure.xlsx
@@ -504,7 +504,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>02:fd:00:05:00:00:00:07:0e:00:00:00:00:00:00</t>
+          <t>0x02:0xfd:0x00:0x05:0x00:0x00:0x00:0x07:0x0e:0x00:0x00:0x00:0x00:0x00:0x00</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -542,7 +542,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>02:fd:00:06:00:00:00:0d:0e:00:e0:00:10:00:00:00:00:00:00:00:00</t>
+          <t>0x02:0xfd:0x00:0x06:0x00:0x00:0x00:0x0d:0x0e:0x00:0xe0:0x00:0x10:0x00:0x00:0x00:0x00:0x00:0x00:0x00:0x00</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -580,7 +580,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>02:fd:00:01:00:00:00:00</t>
+          <t>0x02:0xfd:0x00:0x01:0x00:0x00:0x00:0x00</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -618,7 +618,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>02:fd:00:04:00:00:00:21:31:32:33:34:35:36:37:38:39:30:31:32:33:34:35:36:37:e0:00:e1:e2:e3:e4:e5:e6:a1:a2:a3:a4:a5:a6:00:00</t>
+          <t>0x02:0xfd:0x00:0x04:0x00:0x00:0x00:0x21:0x31:0x32:0x33:0x34:0x35:0x36:0x37:0x38:0x39:0x30:0x31:0x32:0x33:0x34:0x35:0x36:0x37:0xe0:0x00:0xe1:0xe2:0xe3:0xe4:0xe5:0xe6:0xa1:0xa2:0xa3:0xa4:0xa5:0xa6:0x00:0x00</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
@@ -656,12 +656,12 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>02:fd:80:01:00:00:00:06:0e:00:10:32:3e:00</t>
+          <t>0x02:0xfd:0x80:0x01:0x00:0x00:0x00:0x06:0x0e:0x00:0x10:0x32:0x3e:0x00</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>3e:00</t>
+          <t>0x3e:0x00</t>
         </is>
       </c>
     </row>
@@ -694,7 +694,7 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>02:fd:80:02:00:00:00:05:10:32:0e:00:00</t>
+          <t>0x02:0xfd:0x80:0x02:0x00:0x00:0x00:0x05:0x10:0x32:0x0e:0x00:0x00</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
@@ -732,12 +732,12 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>02:fd:80:01:00:00:00:06:10:32:0e:00:7e:00</t>
+          <t>0x02:0xfd:0x80:0x01:0x00:0x00:0x00:0x06:0x10:0x32:0x0e:0x00:0x7e:0x00</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>7e:00</t>
+          <t>0x7e:0x00</t>
         </is>
       </c>
     </row>
@@ -770,12 +770,12 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>02:fd:80:01:00:00:00:06:0e:00:10:32:3e:80</t>
+          <t>0x02:0xfd:0x80:0x01:0x00:0x00:0x00:0x06:0x0e:0x00:0x10:0x32:0x3e:0x80</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>3e:80</t>
+          <t>0x3e:0x80</t>
         </is>
       </c>
     </row>
@@ -808,7 +808,7 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>02:fd:80:02:00:00:00:05:10:32:0e:00:00</t>
+          <t>0x02:0xfd:0x80:0x02:0x00:0x00:0x00:0x05:0x10:0x32:0x0e:0x00:0x00</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
@@ -846,12 +846,12 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>02:fd:80:01:00:00:00:06:10:32:0e:00:7e:80</t>
+          <t>0x02:0xfd:0x80:0x01:0x00:0x00:0x00:0x06:0x10:0x32:0x0e:0x00:0x7e:0x80</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>7e:80</t>
+          <t>0x7e:0x80</t>
         </is>
       </c>
     </row>
@@ -884,12 +884,12 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>02:fd:80:01:00:00:00:07:0e:00:10:32:22:f1:90</t>
+          <t>0x02:0xfd:0x80:0x01:0x00:0x00:0x00:0x07:0x0e:0x00:0x10:0x32:0x22:0xf1:0x90</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>22:f1:90</t>
+          <t>0x22:0xf1:0x90</t>
         </is>
       </c>
     </row>
@@ -922,7 +922,7 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>02:fd:80:02:00:00:00:05:10:32:0e:00:00</t>
+          <t>0x02:0xfd:0x80:0x02:0x00:0x00:0x00:0x05:0x10:0x32:0x0e:0x00:0x00</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
@@ -960,12 +960,12 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>02:fd:80:01:00:00:00:18:10:32:0e:00:62:f1:90:4d:41:54:31:32:33:34:35:36:37:38:39:30:31:32:33:34</t>
+          <t>0x02:0xfd:0x80:0x01:0x00:0x00:0x00:0x18:0x10:0x32:0x0e:0x00:0x62:0xf1:0x90:0x4d:0x41:0x54:0x31:0x32:0x33:0x34:0x35:0x36:0x37:0x38:0x39:0x30:0x31:0x32:0x33:0x34</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>62:f1:90:4d:41:54:31:32:33:34:35:36:37:38:39:30:31:32:33:34</t>
+          <t>0x62:0xf1:0x90:0x4d:0x41:0x54:0x31:0x32:0x33:0x34:0x35:0x36:0x37:0x38:0x39:0x30:0x31:0x32:0x33:0x34</t>
         </is>
       </c>
     </row>
@@ -998,12 +998,12 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>02:fd:80:01:00:00:00:06:0e:00:10:32:10:01</t>
+          <t>0x02:0xfd:0x80:0x01:0x00:0x00:0x00:0x06:0x0e:0x00:0x10:0x32:0x10:0x01</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>10:01</t>
+          <t>0x10:0x01</t>
         </is>
       </c>
     </row>
@@ -1036,7 +1036,7 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>02:fd:80:02:00:00:00:05:10:32:0e:00:00</t>
+          <t>0x02:0xfd:0x80:0x02:0x00:0x00:0x00:0x05:0x10:0x32:0x0e:0x00:0x00</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
@@ -1074,12 +1074,12 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>02:fd:80:01:00:00:00:0a:10:32:0e:00:50:01:00:32:01:f4</t>
+          <t>0x02:0xfd:0x80:0x01:0x00:0x00:0x00:0x0a:0x10:0x32:0x0e:0x00:0x50:0x01:0x00:0x32:0x01:0xf4</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>50:01:00:32:01:f4</t>
+          <t>0x50:0x01:0x00:0x32:0x01:0xf4</t>
         </is>
       </c>
     </row>
@@ -1112,7 +1112,7 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>02:fd:00:05:00:00:00:07:0e:00:00:00:00:00:00</t>
+          <t>0x02:0xfd:0x00:0x05:0x00:0x00:0x00:0x07:0x0e:0x00:0x00:0x00:0x00:0x00:0x00</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
@@ -1150,7 +1150,7 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>02:fd:00:06:00:00:00:0d:0e:00:e0:00:10:00:00:00:00:00:00:00:00</t>
+          <t>0x02:0xfd:0x00:0x06:0x00:0x00:0x00:0x0d:0x0e:0x00:0xe0:0x00:0x10:0x00:0x00:0x00:0x00:0x00:0x00:0x00:0x00</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
@@ -1188,7 +1188,7 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>02:fd:00:01:00:00:00:00</t>
+          <t>0x02:0xfd:0x00:0x01:0x00:0x00:0x00:0x00</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
@@ -1226,7 +1226,7 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>02:fd:00:04:00:00:00:21:31:32:33:34:35:36:37:38:39:30:31:32:33:34:35:36:37:e0:00:e1:e2:e3:e4:e5:e6:a1:a2:a3:a4:a5:a6:00:00</t>
+          <t>0x02:0xfd:0x00:0x04:0x00:0x00:0x00:0x21:0x31:0x32:0x33:0x34:0x35:0x36:0x37:0x38:0x39:0x30:0x31:0x32:0x33:0x34:0x35:0x36:0x37:0xe0:0x00:0xe1:0xe2:0xe3:0xe4:0xe5:0xe6:0xa1:0xa2:0xa3:0xa4:0xa5:0xa6:0x00:0x00</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
@@ -1264,12 +1264,12 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>02:fd:80:01:00:00:00:06:0e:00:e0:01:3e:00</t>
+          <t>0x02:0xfd:0x80:0x01:0x00:0x00:0x00:0x06:0x0e:0x00:0xe0:0x01:0x3e:0x00</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>3e:00</t>
+          <t>0x3e:0x00</t>
         </is>
       </c>
     </row>
@@ -1302,7 +1302,7 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>02:fd:80:02:00:00:00:05:e0:01:0e:00:00</t>
+          <t>0x02:0xfd:0x80:0x02:0x00:0x00:0x00:0x05:0xe0:0x01:0x0e:0x00:0x00</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
@@ -1340,12 +1340,12 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>02:fd:80:01:00:00:00:06:e0:01:0e:00:7e:00</t>
+          <t>0x02:0xfd:0x80:0x01:0x00:0x00:0x00:0x06:0xe0:0x01:0x0e:0x00:0x7e:0x00</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>7e:00</t>
+          <t>0x7e:0x00</t>
         </is>
       </c>
     </row>
@@ -1378,12 +1378,12 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>02:fd:80:01:00:00:00:06:0e:00:e0:01:3e:80</t>
+          <t>0x02:0xfd:0x80:0x01:0x00:0x00:0x00:0x06:0x0e:0x00:0xe0:0x01:0x3e:0x80</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>3e:80</t>
+          <t>0x3e:0x80</t>
         </is>
       </c>
     </row>
@@ -1416,7 +1416,7 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>02:fd:80:02:00:00:00:05:e0:01:0e:00:00</t>
+          <t>0x02:0xfd:0x80:0x02:0x00:0x00:0x00:0x05:0xe0:0x01:0x0e:0x00:0x00</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
@@ -1454,12 +1454,12 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>02:fd:80:01:00:00:00:06:e0:01:0e:00:7e:80</t>
+          <t>0x02:0xfd:0x80:0x01:0x00:0x00:0x00:0x06:0xe0:0x01:0x0e:0x00:0x7e:0x80</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>7e:80</t>
+          <t>0x7e:0x80</t>
         </is>
       </c>
     </row>
@@ -1492,12 +1492,12 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>02:fd:80:01:00:00:00:07:0e:00:e0:01:22:f1:90</t>
+          <t>0x02:0xfd:0x80:0x01:0x00:0x00:0x00:0x07:0x0e:0x00:0xe0:0x01:0x22:0xf1:0x90</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>22:f1:90</t>
+          <t>0x22:0xf1:0x90</t>
         </is>
       </c>
     </row>
@@ -1530,7 +1530,7 @@
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>02:fd:80:02:00:00:00:05:e0:01:0e:00:00</t>
+          <t>0x02:0xfd:0x80:0x02:0x00:0x00:0x00:0x05:0xe0:0x01:0x0e:0x00:0x00</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
@@ -1568,12 +1568,12 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>02:fd:80:01:00:00:00:18:e0:01:0e:00:62:f1:90:4d:41:54:31:32:33:34:35:36:37:38:39:30:31:32:33:34</t>
+          <t>0x02:0xfd:0x80:0x01:0x00:0x00:0x00:0x18:0xe0:0x01:0x0e:0x00:0x62:0xf1:0x90:0x4d:0x41:0x54:0x31:0x32:0x33:0x34:0x35:0x36:0x37:0x38:0x39:0x30:0x31:0x32:0x33:0x34</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>62:f1:90:4d:41:54:31:32:33:34:35:36:37:38:39:30:31:32:33:34</t>
+          <t>0x62:0xf1:0x90:0x4d:0x41:0x54:0x31:0x32:0x33:0x34:0x35:0x36:0x37:0x38:0x39:0x30:0x31:0x32:0x33:0x34</t>
         </is>
       </c>
     </row>
@@ -1606,12 +1606,12 @@
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>02:fd:80:01:00:00:00:06:0e:00:e0:01:10:02</t>
+          <t>0x02:0xfd:0x80:0x01:0x00:0x00:0x00:0x06:0x0e:0x00:0xe0:0x01:0x10:0x02</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>10:02</t>
+          <t>0x10:0x02</t>
         </is>
       </c>
     </row>
@@ -1644,7 +1644,7 @@
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>02:fd:80:02:00:00:00:05:e0:01:0e:00:00</t>
+          <t>0x02:0xfd:0x80:0x02:0x00:0x00:0x00:0x05:0xe0:0x01:0x0e:0x00:0x00</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
@@ -1682,12 +1682,12 @@
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>02:fd:80:01:00:00:00:06:0e:00:e0:01:27:01</t>
+          <t>0x02:0xfd:0x80:0x01:0x00:0x00:0x00:0x06:0x0e:0x00:0xe0:0x01:0x27:0x01</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>27:01</t>
+          <t>0x27:0x01</t>
         </is>
       </c>
     </row>
@@ -1720,7 +1720,7 @@
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>02:fd:80:02:00:00:00:05:e0:01:0e:00:00</t>
+          <t>0x02:0xfd:0x80:0x02:0x00:0x00:0x00:0x05:0xe0:0x01:0x0e:0x00:0x00</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
@@ -1758,12 +1758,12 @@
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>02:fd:80:01:00:00:00:09:e0:01:0e:00:67:01:01:01:01</t>
+          <t>0x02:0xfd:0x80:0x01:0x00:0x00:0x00:0x09:0xe0:0x01:0x0e:0x00:0x67:0x01:0x01:0x01:0x01</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>67:01:01:01:01</t>
+          <t>0x67:0x01:0x01:0x01:0x01</t>
         </is>
       </c>
     </row>
@@ -1796,12 +1796,12 @@
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>02:fd:80:01:00:00:00:06:0e:00:e0:01:27:02</t>
+          <t>0x02:0xfd:0x80:0x01:0x00:0x00:0x00:0x06:0x0e:0x00:0xe0:0x01:0x27:0x02</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>27:02</t>
+          <t>0x27:0x02</t>
         </is>
       </c>
     </row>
@@ -1834,7 +1834,7 @@
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>02:fd:80:02:00:00:00:05:e0:01:0e:00:00</t>
+          <t>0x02:0xfd:0x80:0x02:0x00:0x00:0x00:0x05:0xe0:0x01:0x0e:0x00:0x00</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
@@ -1872,12 +1872,12 @@
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>02:fd:80:01:00:00:00:07:e0:01:0e:00:7f:27:22</t>
+          <t>0x02:0xfd:0x80:0x01:0x00:0x00:0x00:0x07:0xe0:0x01:0x0e:0x00:0x7f:0x27:0x22</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>7f:27:22</t>
+          <t>0x7f:0x27:0x22</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
added functionality to engineer_data.py to capitalize letters in codes for easier lookup. ALso re-output Excel documents with this change
</commit_message>
<xml_diff>
--- a/data/EMSSecurityAccessFailure.xlsx
+++ b/data/EMSSecurityAccessFailure.xlsx
@@ -504,7 +504,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>0x02:0xfd:0x00:0x05:0x00:0x00:0x00:0x07:0x0e:0x00:0x00:0x00:0x00:0x00:0x00</t>
+          <t>0x02:0xFD:0x00:0x05:0x00:0x00:0x00:0x07:0x0E:0x00:0x00:0x00:0x00:0x00:0x00</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -542,7 +542,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>0x02:0xfd:0x00:0x06:0x00:0x00:0x00:0x0d:0x0e:0x00:0xe0:0x00:0x10:0x00:0x00:0x00:0x00:0x00:0x00:0x00:0x00</t>
+          <t>0x02:0xFD:0x00:0x06:0x00:0x00:0x00:0x0D:0x0E:0x00:0xE0:0x00:0x10:0x00:0x00:0x00:0x00:0x00:0x00:0x00:0x00</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -580,7 +580,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>0x02:0xfd:0x00:0x01:0x00:0x00:0x00:0x00</t>
+          <t>0x02:0xFD:0x00:0x01:0x00:0x00:0x00:0x00</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -618,7 +618,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>0x02:0xfd:0x00:0x04:0x00:0x00:0x00:0x21:0x31:0x32:0x33:0x34:0x35:0x36:0x37:0x38:0x39:0x30:0x31:0x32:0x33:0x34:0x35:0x36:0x37:0xe0:0x00:0xe1:0xe2:0xe3:0xe4:0xe5:0xe6:0xa1:0xa2:0xa3:0xa4:0xa5:0xa6:0x00:0x00</t>
+          <t>0x02:0xFD:0x00:0x04:0x00:0x00:0x00:0x21:0x31:0x32:0x33:0x34:0x35:0x36:0x37:0x38:0x39:0x30:0x31:0x32:0x33:0x34:0x35:0x36:0x37:0xE0:0x00:0xE1:0xE2:0xE3:0xE4:0xE5:0xE6:0xA1:0xA2:0xA3:0xA4:0xA5:0xA6:0x00:0x00</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
@@ -656,12 +656,12 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>0x02:0xfd:0x80:0x01:0x00:0x00:0x00:0x06:0x0e:0x00:0x10:0x32:0x3e:0x00</t>
+          <t>0x02:0xFD:0x80:0x01:0x00:0x00:0x00:0x06:0x0E:0x00:0x10:0x32:0x3E:0x00</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>0x3e:0x00</t>
+          <t>0x3E:0x00</t>
         </is>
       </c>
     </row>
@@ -694,7 +694,7 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>0x02:0xfd:0x80:0x02:0x00:0x00:0x00:0x05:0x10:0x32:0x0e:0x00:0x00</t>
+          <t>0x02:0xFD:0x80:0x02:0x00:0x00:0x00:0x05:0x10:0x32:0x0E:0x00:0x00</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
@@ -732,12 +732,12 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>0x02:0xfd:0x80:0x01:0x00:0x00:0x00:0x06:0x10:0x32:0x0e:0x00:0x7e:0x00</t>
+          <t>0x02:0xFD:0x80:0x01:0x00:0x00:0x00:0x06:0x10:0x32:0x0E:0x00:0x7E:0x00</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>0x7e:0x00</t>
+          <t>0x7E:0x00</t>
         </is>
       </c>
     </row>
@@ -770,12 +770,12 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>0x02:0xfd:0x80:0x01:0x00:0x00:0x00:0x06:0x0e:0x00:0x10:0x32:0x3e:0x80</t>
+          <t>0x02:0xFD:0x80:0x01:0x00:0x00:0x00:0x06:0x0E:0x00:0x10:0x32:0x3E:0x80</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>0x3e:0x80</t>
+          <t>0x3E:0x80</t>
         </is>
       </c>
     </row>
@@ -808,7 +808,7 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>0x02:0xfd:0x80:0x02:0x00:0x00:0x00:0x05:0x10:0x32:0x0e:0x00:0x00</t>
+          <t>0x02:0xFD:0x80:0x02:0x00:0x00:0x00:0x05:0x10:0x32:0x0E:0x00:0x00</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
@@ -846,12 +846,12 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>0x02:0xfd:0x80:0x01:0x00:0x00:0x00:0x06:0x10:0x32:0x0e:0x00:0x7e:0x80</t>
+          <t>0x02:0xFD:0x80:0x01:0x00:0x00:0x00:0x06:0x10:0x32:0x0E:0x00:0x7E:0x80</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>0x7e:0x80</t>
+          <t>0x7E:0x80</t>
         </is>
       </c>
     </row>
@@ -884,12 +884,12 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>0x02:0xfd:0x80:0x01:0x00:0x00:0x00:0x07:0x0e:0x00:0x10:0x32:0x22:0xf1:0x90</t>
+          <t>0x02:0xFD:0x80:0x01:0x00:0x00:0x00:0x07:0x0E:0x00:0x10:0x32:0x22:0xF1:0x90</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>0x22:0xf1:0x90</t>
+          <t>0x22:0xF1:0x90</t>
         </is>
       </c>
     </row>
@@ -922,7 +922,7 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>0x02:0xfd:0x80:0x02:0x00:0x00:0x00:0x05:0x10:0x32:0x0e:0x00:0x00</t>
+          <t>0x02:0xFD:0x80:0x02:0x00:0x00:0x00:0x05:0x10:0x32:0x0E:0x00:0x00</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
@@ -960,12 +960,12 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>0x02:0xfd:0x80:0x01:0x00:0x00:0x00:0x18:0x10:0x32:0x0e:0x00:0x62:0xf1:0x90:0x4d:0x41:0x54:0x31:0x32:0x33:0x34:0x35:0x36:0x37:0x38:0x39:0x30:0x31:0x32:0x33:0x34</t>
+          <t>0x02:0xFD:0x80:0x01:0x00:0x00:0x00:0x18:0x10:0x32:0x0E:0x00:0x62:0xF1:0x90:0x4D:0x41:0x54:0x31:0x32:0x33:0x34:0x35:0x36:0x37:0x38:0x39:0x30:0x31:0x32:0x33:0x34</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>0x62:0xf1:0x90:0x4d:0x41:0x54:0x31:0x32:0x33:0x34:0x35:0x36:0x37:0x38:0x39:0x30:0x31:0x32:0x33:0x34</t>
+          <t>0x62:0xF1:0x90:0x4D:0x41:0x54:0x31:0x32:0x33:0x34:0x35:0x36:0x37:0x38:0x39:0x30:0x31:0x32:0x33:0x34</t>
         </is>
       </c>
     </row>
@@ -998,7 +998,7 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>0x02:0xfd:0x80:0x01:0x00:0x00:0x00:0x06:0x0e:0x00:0x10:0x32:0x10:0x01</t>
+          <t>0x02:0xFD:0x80:0x01:0x00:0x00:0x00:0x06:0x0E:0x00:0x10:0x32:0x10:0x01</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
@@ -1036,7 +1036,7 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>0x02:0xfd:0x80:0x02:0x00:0x00:0x00:0x05:0x10:0x32:0x0e:0x00:0x00</t>
+          <t>0x02:0xFD:0x80:0x02:0x00:0x00:0x00:0x05:0x10:0x32:0x0E:0x00:0x00</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
@@ -1074,12 +1074,12 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>0x02:0xfd:0x80:0x01:0x00:0x00:0x00:0x0a:0x10:0x32:0x0e:0x00:0x50:0x01:0x00:0x32:0x01:0xf4</t>
+          <t>0x02:0xFD:0x80:0x01:0x00:0x00:0x00:0x0A:0x10:0x32:0x0E:0x00:0x50:0x01:0x00:0x32:0x01:0xF4</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>0x50:0x01:0x00:0x32:0x01:0xf4</t>
+          <t>0x50:0x01:0x00:0x32:0x01:0xF4</t>
         </is>
       </c>
     </row>
@@ -1112,7 +1112,7 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>0x02:0xfd:0x00:0x05:0x00:0x00:0x00:0x07:0x0e:0x00:0x00:0x00:0x00:0x00:0x00</t>
+          <t>0x02:0xFD:0x00:0x05:0x00:0x00:0x00:0x07:0x0E:0x00:0x00:0x00:0x00:0x00:0x00</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
@@ -1150,7 +1150,7 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>0x02:0xfd:0x00:0x06:0x00:0x00:0x00:0x0d:0x0e:0x00:0xe0:0x00:0x10:0x00:0x00:0x00:0x00:0x00:0x00:0x00:0x00</t>
+          <t>0x02:0xFD:0x00:0x06:0x00:0x00:0x00:0x0D:0x0E:0x00:0xE0:0x00:0x10:0x00:0x00:0x00:0x00:0x00:0x00:0x00:0x00</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
@@ -1188,7 +1188,7 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>0x02:0xfd:0x00:0x01:0x00:0x00:0x00:0x00</t>
+          <t>0x02:0xFD:0x00:0x01:0x00:0x00:0x00:0x00</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
@@ -1226,7 +1226,7 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>0x02:0xfd:0x00:0x04:0x00:0x00:0x00:0x21:0x31:0x32:0x33:0x34:0x35:0x36:0x37:0x38:0x39:0x30:0x31:0x32:0x33:0x34:0x35:0x36:0x37:0xe0:0x00:0xe1:0xe2:0xe3:0xe4:0xe5:0xe6:0xa1:0xa2:0xa3:0xa4:0xa5:0xa6:0x00:0x00</t>
+          <t>0x02:0xFD:0x00:0x04:0x00:0x00:0x00:0x21:0x31:0x32:0x33:0x34:0x35:0x36:0x37:0x38:0x39:0x30:0x31:0x32:0x33:0x34:0x35:0x36:0x37:0xE0:0x00:0xE1:0xE2:0xE3:0xE4:0xE5:0xE6:0xA1:0xA2:0xA3:0xA4:0xA5:0xA6:0x00:0x00</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
@@ -1264,12 +1264,12 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>0x02:0xfd:0x80:0x01:0x00:0x00:0x00:0x06:0x0e:0x00:0xe0:0x01:0x3e:0x00</t>
+          <t>0x02:0xFD:0x80:0x01:0x00:0x00:0x00:0x06:0x0E:0x00:0xE0:0x01:0x3E:0x00</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>0x3e:0x00</t>
+          <t>0x3E:0x00</t>
         </is>
       </c>
     </row>
@@ -1302,7 +1302,7 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>0x02:0xfd:0x80:0x02:0x00:0x00:0x00:0x05:0xe0:0x01:0x0e:0x00:0x00</t>
+          <t>0x02:0xFD:0x80:0x02:0x00:0x00:0x00:0x05:0xE0:0x01:0x0E:0x00:0x00</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
@@ -1340,12 +1340,12 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>0x02:0xfd:0x80:0x01:0x00:0x00:0x00:0x06:0xe0:0x01:0x0e:0x00:0x7e:0x00</t>
+          <t>0x02:0xFD:0x80:0x01:0x00:0x00:0x00:0x06:0xE0:0x01:0x0E:0x00:0x7E:0x00</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>0x7e:0x00</t>
+          <t>0x7E:0x00</t>
         </is>
       </c>
     </row>
@@ -1378,12 +1378,12 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>0x02:0xfd:0x80:0x01:0x00:0x00:0x00:0x06:0x0e:0x00:0xe0:0x01:0x3e:0x80</t>
+          <t>0x02:0xFD:0x80:0x01:0x00:0x00:0x00:0x06:0x0E:0x00:0xE0:0x01:0x3E:0x80</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>0x3e:0x80</t>
+          <t>0x3E:0x80</t>
         </is>
       </c>
     </row>
@@ -1416,7 +1416,7 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>0x02:0xfd:0x80:0x02:0x00:0x00:0x00:0x05:0xe0:0x01:0x0e:0x00:0x00</t>
+          <t>0x02:0xFD:0x80:0x02:0x00:0x00:0x00:0x05:0xE0:0x01:0x0E:0x00:0x00</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
@@ -1454,12 +1454,12 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>0x02:0xfd:0x80:0x01:0x00:0x00:0x00:0x06:0xe0:0x01:0x0e:0x00:0x7e:0x80</t>
+          <t>0x02:0xFD:0x80:0x01:0x00:0x00:0x00:0x06:0xE0:0x01:0x0E:0x00:0x7E:0x80</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>0x7e:0x80</t>
+          <t>0x7E:0x80</t>
         </is>
       </c>
     </row>
@@ -1492,12 +1492,12 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>0x02:0xfd:0x80:0x01:0x00:0x00:0x00:0x07:0x0e:0x00:0xe0:0x01:0x22:0xf1:0x90</t>
+          <t>0x02:0xFD:0x80:0x01:0x00:0x00:0x00:0x07:0x0E:0x00:0xE0:0x01:0x22:0xF1:0x90</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>0x22:0xf1:0x90</t>
+          <t>0x22:0xF1:0x90</t>
         </is>
       </c>
     </row>
@@ -1530,7 +1530,7 @@
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>0x02:0xfd:0x80:0x02:0x00:0x00:0x00:0x05:0xe0:0x01:0x0e:0x00:0x00</t>
+          <t>0x02:0xFD:0x80:0x02:0x00:0x00:0x00:0x05:0xE0:0x01:0x0E:0x00:0x00</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
@@ -1568,12 +1568,12 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>0x02:0xfd:0x80:0x01:0x00:0x00:0x00:0x18:0xe0:0x01:0x0e:0x00:0x62:0xf1:0x90:0x4d:0x41:0x54:0x31:0x32:0x33:0x34:0x35:0x36:0x37:0x38:0x39:0x30:0x31:0x32:0x33:0x34</t>
+          <t>0x02:0xFD:0x80:0x01:0x00:0x00:0x00:0x18:0xE0:0x01:0x0E:0x00:0x62:0xF1:0x90:0x4D:0x41:0x54:0x31:0x32:0x33:0x34:0x35:0x36:0x37:0x38:0x39:0x30:0x31:0x32:0x33:0x34</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>0x62:0xf1:0x90:0x4d:0x41:0x54:0x31:0x32:0x33:0x34:0x35:0x36:0x37:0x38:0x39:0x30:0x31:0x32:0x33:0x34</t>
+          <t>0x62:0xF1:0x90:0x4D:0x41:0x54:0x31:0x32:0x33:0x34:0x35:0x36:0x37:0x38:0x39:0x30:0x31:0x32:0x33:0x34</t>
         </is>
       </c>
     </row>
@@ -1606,7 +1606,7 @@
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>0x02:0xfd:0x80:0x01:0x00:0x00:0x00:0x06:0x0e:0x00:0xe0:0x01:0x10:0x02</t>
+          <t>0x02:0xFD:0x80:0x01:0x00:0x00:0x00:0x06:0x0E:0x00:0xE0:0x01:0x10:0x02</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
@@ -1644,7 +1644,7 @@
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>0x02:0xfd:0x80:0x02:0x00:0x00:0x00:0x05:0xe0:0x01:0x0e:0x00:0x00</t>
+          <t>0x02:0xFD:0x80:0x02:0x00:0x00:0x00:0x05:0xE0:0x01:0x0E:0x00:0x00</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
@@ -1682,7 +1682,7 @@
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>0x02:0xfd:0x80:0x01:0x00:0x00:0x00:0x06:0x0e:0x00:0xe0:0x01:0x27:0x01</t>
+          <t>0x02:0xFD:0x80:0x01:0x00:0x00:0x00:0x06:0x0E:0x00:0xE0:0x01:0x27:0x01</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
@@ -1720,7 +1720,7 @@
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>0x02:0xfd:0x80:0x02:0x00:0x00:0x00:0x05:0xe0:0x01:0x0e:0x00:0x00</t>
+          <t>0x02:0xFD:0x80:0x02:0x00:0x00:0x00:0x05:0xE0:0x01:0x0E:0x00:0x00</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
@@ -1758,7 +1758,7 @@
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>0x02:0xfd:0x80:0x01:0x00:0x00:0x00:0x09:0xe0:0x01:0x0e:0x00:0x67:0x01:0x01:0x01:0x01</t>
+          <t>0x02:0xFD:0x80:0x01:0x00:0x00:0x00:0x09:0xE0:0x01:0x0E:0x00:0x67:0x01:0x01:0x01:0x01</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
@@ -1796,7 +1796,7 @@
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>0x02:0xfd:0x80:0x01:0x00:0x00:0x00:0x06:0x0e:0x00:0xe0:0x01:0x27:0x02</t>
+          <t>0x02:0xFD:0x80:0x01:0x00:0x00:0x00:0x06:0x0E:0x00:0xE0:0x01:0x27:0x02</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
@@ -1834,7 +1834,7 @@
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>0x02:0xfd:0x80:0x02:0x00:0x00:0x00:0x05:0xe0:0x01:0x0e:0x00:0x00</t>
+          <t>0x02:0xFD:0x80:0x02:0x00:0x00:0x00:0x05:0xE0:0x01:0x0E:0x00:0x00</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
@@ -1872,12 +1872,12 @@
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>0x02:0xfd:0x80:0x01:0x00:0x00:0x00:0x07:0xe0:0x01:0x0e:0x00:0x7f:0x27:0x22</t>
+          <t>0x02:0xFD:0x80:0x01:0x00:0x00:0x00:0x07:0xE0:0x01:0x0E:0x00:0x7F:0x27:0x22</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>0x7f:0x27:0x22</t>
+          <t>0x7F:0x27:0x22</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
updated engineer_data.py and all outputted files to generate sid and reply columns, rather than combination of two in monolithic "uds" column
</commit_message>
<xml_diff>
--- a/data/EMSSecurityAccessFailure.xlsx
+++ b/data/EMSSecurityAccessFailure.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H38"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,13 +471,18 @@
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>uds</t>
+          <t>sid</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>reply</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -486,11 +491,11 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>DOIP</t>
+          <t>UDS</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -499,23 +504,28 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>0x1032</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>0x02:0xFD:0x00:0x05:0x00:0x00:0x00:0x07:0x0E:0x00:0x00:0x00:0x00:0x00:0x00</t>
+          <t>0x02:0xFD:0x80:0x01:0x00:0x00:0x00:0x06:0x0E:0x00:0x10:0x32:0x3E:0x00</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>0x3E</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>0x00</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -524,36 +534,41 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>DOIP</t>
+          <t>UDS</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>0xe000</t>
+          <t>0x1032</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>0x0e00</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>0x02:0xFD:0x00:0x06:0x00:0x00:0x00:0x0D:0x0E:0x00:0xE0:0x00:0x10:0x00:0x00:0x00:0x00:0x00:0x00:0x00:0x00</t>
+          <t>0x02:0xFD:0x80:0x01:0x00:0x00:0x00:0x06:0x10:0x32:0x0E:0x00:0x7E:0x00</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>0x3E</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>0x01</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -562,36 +577,41 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>DOIP</t>
+          <t>UDS</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>0x0e00</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>0x1032</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>0x02:0xFD:0x00:0x01:0x00:0x00:0x00:0x00</t>
+          <t>0x02:0xFD:0x80:0x01:0x00:0x00:0x00:0x06:0x0E:0x00:0x10:0x32:0x3E:0x80</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>0x3E</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>0x00</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -600,36 +620,41 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>DOIP</t>
+          <t>UDS</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>0x1032</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>0x0e00</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>0x02:0xFD:0x00:0x04:0x00:0x00:0x00:0x21:0x31:0x32:0x33:0x34:0x35:0x36:0x37:0x38:0x39:0x30:0x31:0x32:0x33:0x34:0x35:0x36:0x37:0xE0:0x00:0xE1:0xE2:0xE3:0xE4:0xE5:0xE6:0xA1:0xA2:0xA3:0xA4:0xA5:0xA6:0x00:0x00</t>
+          <t>0x02:0xFD:0x80:0x01:0x00:0x00:0x00:0x06:0x10:0x32:0x0E:0x00:0x7E:0x80</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>0x3E</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>0x01</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -642,7 +667,7 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -656,18 +681,23 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>0x02:0xFD:0x80:0x01:0x00:0x00:0x00:0x06:0x0E:0x00:0x10:0x32:0x3E:0x00</t>
+          <t>0x02:0xFD:0x80:0x01:0x00:0x00:0x00:0x07:0x0E:0x00:0x10:0x32:0x22:0xF1:0x90</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>0x3E:0x00</t>
+          <t>0x22</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>0x00</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -676,11 +706,11 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>DOIP</t>
+          <t>UDS</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>79</v>
+        <v>98</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -694,18 +724,23 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>0x02:0xFD:0x80:0x02:0x00:0x00:0x00:0x05:0x10:0x32:0x0E:0x00:0x00</t>
+          <t>0x02:0xFD:0x80:0x01:0x00:0x00:0x00:0x18:0x10:0x32:0x0E:0x00:0x62:0xF1:0x90:0x4D:0x41:0x54:0x31:0x32:0x33:0x34:0x35:0x36:0x37:0x38:0x39:0x30:0x31:0x32:0x33:0x34</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>0x22</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>0x01</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -722,28 +757,33 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
+          <t>0x0e00</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
           <t>0x1032</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>0x0e00</t>
-        </is>
-      </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>0x02:0xFD:0x80:0x01:0x00:0x00:0x00:0x06:0x10:0x32:0x0E:0x00:0x7E:0x00</t>
+          <t>0x02:0xFD:0x80:0x01:0x00:0x00:0x00:0x06:0x0E:0x00:0x10:0x32:0x10:0x01</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>0x7E:0x00</t>
+          <t>0x10</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>0x00</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -756,32 +796,37 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>0x0e00</t>
+          <t>0x1032</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>0x1032</t>
+          <t>0x0e00</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>0x02:0xFD:0x80:0x01:0x00:0x00:0x00:0x06:0x0E:0x00:0x10:0x32:0x3E:0x80</t>
+          <t>0x02:0xFD:0x80:0x01:0x00:0x00:0x00:0x0A:0x10:0x32:0x0E:0x00:0x50:0x01:0x00:0x32:0x01:0xF4</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>0x3E:0x80</t>
+          <t>0x10</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>0x01</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -790,36 +835,41 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>DOIP</t>
+          <t>UDS</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>0x1032</t>
+          <t>0x0e00</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>0x0e00</t>
+          <t>0xe001</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>0x02:0xFD:0x80:0x02:0x00:0x00:0x00:0x05:0x10:0x32:0x0E:0x00:0x00</t>
+          <t>0x02:0xFD:0x80:0x01:0x00:0x00:0x00:0x06:0x0E:0x00:0xE0:0x01:0x3E:0x00</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>0x3E</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>0x00</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -836,7 +886,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>0x1032</t>
+          <t>0xe001</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -846,18 +896,23 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>0x02:0xFD:0x80:0x01:0x00:0x00:0x00:0x06:0x10:0x32:0x0E:0x00:0x7E:0x80</t>
+          <t>0x02:0xFD:0x80:0x01:0x00:0x00:0x00:0x06:0xE0:0x01:0x0E:0x00:0x7E:0x00</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>0x7E:0x80</t>
+          <t>0x3E</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>0x01</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
@@ -870,7 +925,7 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -879,23 +934,28 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>0x1032</t>
+          <t>0xe001</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>0x02:0xFD:0x80:0x01:0x00:0x00:0x00:0x07:0x0E:0x00:0x10:0x32:0x22:0xF1:0x90</t>
+          <t>0x02:0xFD:0x80:0x01:0x00:0x00:0x00:0x06:0x0E:0x00:0xE0:0x01:0x3E:0x80</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>0x22:0xF1:0x90</t>
+          <t>0x3E</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>0x00</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>19</v>
+        <v>44</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
@@ -904,15 +964,15 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>DOIP</t>
+          <t>UDS</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>0x1032</t>
+          <t>0xe001</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -922,18 +982,23 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>0x02:0xFD:0x80:0x02:0x00:0x00:0x00:0x05:0x10:0x32:0x0E:0x00:0x00</t>
+          <t>0x02:0xFD:0x80:0x01:0x00:0x00:0x00:0x06:0xE0:0x01:0x0E:0x00:0x7E:0x80</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>0x3E</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>0x01</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
@@ -946,32 +1011,37 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>0x1032</t>
+          <t>0x0e00</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>0x0e00</t>
+          <t>0xe001</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>0x02:0xFD:0x80:0x01:0x00:0x00:0x00:0x18:0x10:0x32:0x0E:0x00:0x62:0xF1:0x90:0x4D:0x41:0x54:0x31:0x32:0x33:0x34:0x35:0x36:0x37:0x38:0x39:0x30:0x31:0x32:0x33:0x34</t>
+          <t>0x02:0xFD:0x80:0x01:0x00:0x00:0x00:0x07:0x0E:0x00:0xE0:0x01:0x22:0xF1:0x90</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>0x62:0xF1:0x90:0x4D:0x41:0x54:0x31:0x32:0x33:0x34:0x35:0x36:0x37:0x38:0x39:0x30:0x31:0x32:0x33:0x34</t>
+          <t>0x22</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>0x00</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>22</v>
+        <v>48</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
@@ -984,32 +1054,37 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>80</v>
+        <v>98</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>0x0e00</t>
+          <t>0xe001</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>0x1032</t>
+          <t>0x0e00</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>0x02:0xFD:0x80:0x01:0x00:0x00:0x00:0x06:0x0E:0x00:0x10:0x32:0x10:0x01</t>
+          <t>0x02:0xFD:0x80:0x01:0x00:0x00:0x00:0x18:0xE0:0x01:0x0E:0x00:0x62:0xF1:0x90:0x4D:0x41:0x54:0x31:0x32:0x33:0x34:0x35:0x36:0x37:0x38:0x39:0x30:0x31:0x32:0x33:0x34</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>0x10:0x01</t>
+          <t>0x22</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>0x01</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>23</v>
+        <v>50</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
@@ -1018,36 +1093,41 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>DOIP</t>
+          <t>UDS</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>0x1032</t>
+          <t>0x0e00</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>0x0e00</t>
+          <t>0xe001</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>0x02:0xFD:0x80:0x02:0x00:0x00:0x00:0x05:0x10:0x32:0x0E:0x00:0x00</t>
+          <t>0x02:0xFD:0x80:0x01:0x00:0x00:0x00:0x06:0x0E:0x00:0xE0:0x01:0x10:0x02</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>0x10</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>0x00</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>24</v>
+        <v>54</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
@@ -1060,32 +1140,37 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>0x1032</t>
+          <t>0x0e00</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>0x0e00</t>
+          <t>0xe001</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>0x02:0xFD:0x80:0x01:0x00:0x00:0x00:0x0A:0x10:0x32:0x0E:0x00:0x50:0x01:0x00:0x32:0x01:0xF4</t>
+          <t>0x02:0xFD:0x80:0x01:0x00:0x00:0x00:0x06:0x0E:0x00:0xE0:0x01:0x27:0x01</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>0x50:0x01:0x00:0x32:0x01:0xF4</t>
+          <t>0x27</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>0x00</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>32</v>
+        <v>56</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
@@ -1094,36 +1179,41 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>DOIP</t>
+          <t>UDS</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>0x0e00</t>
+          <t>0xe001</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>0x0e00</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>0x02:0xFD:0x00:0x05:0x00:0x00:0x00:0x07:0x0E:0x00:0x00:0x00:0x00:0x00:0x00</t>
+          <t>0x02:0xFD:0x80:0x01:0x00:0x00:0x00:0x09:0xE0:0x01:0x0E:0x00:0x67:0x01:0x01:0x01:0x01</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>0x27</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>0x01</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>34</v>
+        <v>58</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
@@ -1132,36 +1222,41 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>DOIP</t>
+          <t>UDS</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>0xe000</t>
+          <t>0x0e00</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>0xe001</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>0x02:0xFD:0x00:0x06:0x00:0x00:0x00:0x0D:0x0E:0x00:0xE0:0x00:0x10:0x00:0x00:0x00:0x00:0x00:0x00:0x00:0x00</t>
+          <t>0x02:0xFD:0x80:0x01:0x00:0x00:0x00:0x06:0x0E:0x00:0xE0:0x01:0x27:0x02</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>0x27</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>0x00</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>36</v>
+        <v>60</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
@@ -1170,714 +1265,35 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>DOIP</t>
+          <t>UDS</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>50</v>
+        <v>81</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>0xe001</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>0x0e00</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>0x02:0xFD:0x00:0x01:0x00:0x00:0x00:0x00</t>
+          <t>0x02:0xFD:0x80:0x01:0x00:0x00:0x00:0x07:0xE0:0x01:0x0E:0x00:0x7F:0x27:0x22</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="n">
-        <v>37</v>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>2024-09-18 11:35:32</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>DOIP</t>
-        </is>
-      </c>
-      <c r="D21" t="n">
-        <v>83</v>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>0x02:0xFD:0x00:0x04:0x00:0x00:0x00:0x21:0x31:0x32:0x33:0x34:0x35:0x36:0x37:0x38:0x39:0x30:0x31:0x32:0x33:0x34:0x35:0x36:0x37:0xE0:0x00:0xE1:0xE2:0xE3:0xE4:0xE5:0xE6:0xA1:0xA2:0xA3:0xA4:0xA5:0xA6:0x00:0x00</t>
-        </is>
-      </c>
-      <c r="H21" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="n">
-        <v>38</v>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>2024-09-18 11:35:32</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>UDS</t>
-        </is>
-      </c>
-      <c r="D22" t="n">
-        <v>80</v>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>0x0e00</t>
-        </is>
-      </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>0xe001</t>
-        </is>
-      </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>0x02:0xFD:0x80:0x01:0x00:0x00:0x00:0x06:0x0E:0x00:0xE0:0x01:0x3E:0x00</t>
-        </is>
-      </c>
-      <c r="H22" t="inlineStr">
-        <is>
-          <t>0x3E:0x00</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="n">
-        <v>39</v>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>2024-09-18 11:35:32</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>DOIP</t>
-        </is>
-      </c>
-      <c r="D23" t="n">
-        <v>79</v>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>0xe001</t>
-        </is>
-      </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>0x0e00</t>
-        </is>
-      </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>0x02:0xFD:0x80:0x02:0x00:0x00:0x00:0x05:0xE0:0x01:0x0E:0x00:0x00</t>
-        </is>
-      </c>
-      <c r="H23" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="n">
-        <v>40</v>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>2024-09-18 11:35:32</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>UDS</t>
-        </is>
-      </c>
-      <c r="D24" t="n">
-        <v>80</v>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>0xe001</t>
-        </is>
-      </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>0x0e00</t>
-        </is>
-      </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>0x02:0xFD:0x80:0x01:0x00:0x00:0x00:0x06:0xE0:0x01:0x0E:0x00:0x7E:0x00</t>
-        </is>
-      </c>
-      <c r="H24" t="inlineStr">
-        <is>
-          <t>0x7E:0x00</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="n">
-        <v>42</v>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>2024-09-18 11:35:32</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>UDS</t>
-        </is>
-      </c>
-      <c r="D25" t="n">
-        <v>80</v>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>0x0e00</t>
-        </is>
-      </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>0xe001</t>
-        </is>
-      </c>
-      <c r="G25" t="inlineStr">
-        <is>
-          <t>0x02:0xFD:0x80:0x01:0x00:0x00:0x00:0x06:0x0E:0x00:0xE0:0x01:0x3E:0x80</t>
-        </is>
-      </c>
-      <c r="H25" t="inlineStr">
-        <is>
-          <t>0x3E:0x80</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="n">
-        <v>43</v>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>2024-09-18 11:35:32</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>DOIP</t>
-        </is>
-      </c>
-      <c r="D26" t="n">
-        <v>79</v>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>0xe001</t>
-        </is>
-      </c>
-      <c r="F26" t="inlineStr">
-        <is>
-          <t>0x0e00</t>
-        </is>
-      </c>
-      <c r="G26" t="inlineStr">
-        <is>
-          <t>0x02:0xFD:0x80:0x02:0x00:0x00:0x00:0x05:0xE0:0x01:0x0E:0x00:0x00</t>
-        </is>
-      </c>
-      <c r="H26" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="n">
-        <v>44</v>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>2024-09-18 11:35:32</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>UDS</t>
-        </is>
-      </c>
-      <c r="D27" t="n">
-        <v>80</v>
-      </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>0xe001</t>
-        </is>
-      </c>
-      <c r="F27" t="inlineStr">
-        <is>
-          <t>0x0e00</t>
-        </is>
-      </c>
-      <c r="G27" t="inlineStr">
-        <is>
-          <t>0x02:0xFD:0x80:0x01:0x00:0x00:0x00:0x06:0xE0:0x01:0x0E:0x00:0x7E:0x80</t>
-        </is>
-      </c>
-      <c r="H27" t="inlineStr">
-        <is>
-          <t>0x7E:0x80</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="n">
-        <v>46</v>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>2024-09-18 11:35:32</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>UDS</t>
-        </is>
-      </c>
-      <c r="D28" t="n">
-        <v>81</v>
-      </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>0x0e00</t>
-        </is>
-      </c>
-      <c r="F28" t="inlineStr">
-        <is>
-          <t>0xe001</t>
-        </is>
-      </c>
-      <c r="G28" t="inlineStr">
-        <is>
-          <t>0x02:0xFD:0x80:0x01:0x00:0x00:0x00:0x07:0x0E:0x00:0xE0:0x01:0x22:0xF1:0x90</t>
-        </is>
-      </c>
-      <c r="H28" t="inlineStr">
-        <is>
-          <t>0x22:0xF1:0x90</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="n">
-        <v>47</v>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>2024-09-18 11:35:32</t>
-        </is>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>DOIP</t>
-        </is>
-      </c>
-      <c r="D29" t="n">
-        <v>79</v>
-      </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>0xe001</t>
-        </is>
-      </c>
-      <c r="F29" t="inlineStr">
-        <is>
-          <t>0x0e00</t>
-        </is>
-      </c>
-      <c r="G29" t="inlineStr">
-        <is>
-          <t>0x02:0xFD:0x80:0x02:0x00:0x00:0x00:0x05:0xE0:0x01:0x0E:0x00:0x00</t>
-        </is>
-      </c>
-      <c r="H29" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="n">
-        <v>48</v>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>2024-09-18 11:35:32</t>
-        </is>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>UDS</t>
-        </is>
-      </c>
-      <c r="D30" t="n">
-        <v>98</v>
-      </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>0xe001</t>
-        </is>
-      </c>
-      <c r="F30" t="inlineStr">
-        <is>
-          <t>0x0e00</t>
-        </is>
-      </c>
-      <c r="G30" t="inlineStr">
-        <is>
-          <t>0x02:0xFD:0x80:0x01:0x00:0x00:0x00:0x18:0xE0:0x01:0x0E:0x00:0x62:0xF1:0x90:0x4D:0x41:0x54:0x31:0x32:0x33:0x34:0x35:0x36:0x37:0x38:0x39:0x30:0x31:0x32:0x33:0x34</t>
-        </is>
-      </c>
-      <c r="H30" t="inlineStr">
-        <is>
-          <t>0x62:0xF1:0x90:0x4D:0x41:0x54:0x31:0x32:0x33:0x34:0x35:0x36:0x37:0x38:0x39:0x30:0x31:0x32:0x33:0x34</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="n">
-        <v>50</v>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>2024-09-18 11:35:32</t>
-        </is>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>UDS</t>
-        </is>
-      </c>
-      <c r="D31" t="n">
-        <v>80</v>
-      </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>0x0e00</t>
-        </is>
-      </c>
-      <c r="F31" t="inlineStr">
-        <is>
-          <t>0xe001</t>
-        </is>
-      </c>
-      <c r="G31" t="inlineStr">
-        <is>
-          <t>0x02:0xFD:0x80:0x01:0x00:0x00:0x00:0x06:0x0E:0x00:0xE0:0x01:0x10:0x02</t>
-        </is>
-      </c>
-      <c r="H31" t="inlineStr">
-        <is>
-          <t>0x10:0x02</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="n">
-        <v>51</v>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>2024-09-18 11:35:32</t>
-        </is>
-      </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>DOIP</t>
-        </is>
-      </c>
-      <c r="D32" t="n">
-        <v>79</v>
-      </c>
-      <c r="E32" t="inlineStr">
-        <is>
-          <t>0xe001</t>
-        </is>
-      </c>
-      <c r="F32" t="inlineStr">
-        <is>
-          <t>0x0e00</t>
-        </is>
-      </c>
-      <c r="G32" t="inlineStr">
-        <is>
-          <t>0x02:0xFD:0x80:0x02:0x00:0x00:0x00:0x05:0xE0:0x01:0x0E:0x00:0x00</t>
-        </is>
-      </c>
-      <c r="H32" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="n">
-        <v>54</v>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>2024-09-18 11:35:32</t>
-        </is>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>UDS</t>
-        </is>
-      </c>
-      <c r="D33" t="n">
-        <v>80</v>
-      </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>0x0e00</t>
-        </is>
-      </c>
-      <c r="F33" t="inlineStr">
-        <is>
-          <t>0xe001</t>
-        </is>
-      </c>
-      <c r="G33" t="inlineStr">
-        <is>
-          <t>0x02:0xFD:0x80:0x01:0x00:0x00:0x00:0x06:0x0E:0x00:0xE0:0x01:0x27:0x01</t>
-        </is>
-      </c>
-      <c r="H33" t="inlineStr">
-        <is>
-          <t>0x27:0x01</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="n">
-        <v>55</v>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>2024-09-18 11:35:32</t>
-        </is>
-      </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>DOIP</t>
-        </is>
-      </c>
-      <c r="D34" t="n">
-        <v>79</v>
-      </c>
-      <c r="E34" t="inlineStr">
-        <is>
-          <t>0xe001</t>
-        </is>
-      </c>
-      <c r="F34" t="inlineStr">
-        <is>
-          <t>0x0e00</t>
-        </is>
-      </c>
-      <c r="G34" t="inlineStr">
-        <is>
-          <t>0x02:0xFD:0x80:0x02:0x00:0x00:0x00:0x05:0xE0:0x01:0x0E:0x00:0x00</t>
-        </is>
-      </c>
-      <c r="H34" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="n">
-        <v>56</v>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>2024-09-18 11:35:32</t>
-        </is>
-      </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>UDS</t>
-        </is>
-      </c>
-      <c r="D35" t="n">
-        <v>83</v>
-      </c>
-      <c r="E35" t="inlineStr">
-        <is>
-          <t>0xe001</t>
-        </is>
-      </c>
-      <c r="F35" t="inlineStr">
-        <is>
-          <t>0x0e00</t>
-        </is>
-      </c>
-      <c r="G35" t="inlineStr">
-        <is>
-          <t>0x02:0xFD:0x80:0x01:0x00:0x00:0x00:0x09:0xE0:0x01:0x0E:0x00:0x67:0x01:0x01:0x01:0x01</t>
-        </is>
-      </c>
-      <c r="H35" t="inlineStr">
-        <is>
-          <t>0x67:0x01:0x01:0x01:0x01</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="n">
-        <v>58</v>
-      </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>2024-09-18 11:35:32</t>
-        </is>
-      </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>UDS</t>
-        </is>
-      </c>
-      <c r="D36" t="n">
-        <v>80</v>
-      </c>
-      <c r="E36" t="inlineStr">
-        <is>
-          <t>0x0e00</t>
-        </is>
-      </c>
-      <c r="F36" t="inlineStr">
-        <is>
-          <t>0xe001</t>
-        </is>
-      </c>
-      <c r="G36" t="inlineStr">
-        <is>
-          <t>0x02:0xFD:0x80:0x01:0x00:0x00:0x00:0x06:0x0E:0x00:0xE0:0x01:0x27:0x02</t>
-        </is>
-      </c>
-      <c r="H36" t="inlineStr">
-        <is>
-          <t>0x27:0x02</t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="n">
-        <v>59</v>
-      </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>2024-09-18 11:35:32</t>
-        </is>
-      </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>DOIP</t>
-        </is>
-      </c>
-      <c r="D37" t="n">
-        <v>79</v>
-      </c>
-      <c r="E37" t="inlineStr">
-        <is>
-          <t>0xe001</t>
-        </is>
-      </c>
-      <c r="F37" t="inlineStr">
-        <is>
-          <t>0x0e00</t>
-        </is>
-      </c>
-      <c r="G37" t="inlineStr">
-        <is>
-          <t>0x02:0xFD:0x80:0x02:0x00:0x00:0x00:0x05:0xE0:0x01:0x0E:0x00:0x00</t>
-        </is>
-      </c>
-      <c r="H37" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="n">
-        <v>60</v>
-      </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>2024-09-18 11:35:32</t>
-        </is>
-      </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>UDS</t>
-        </is>
-      </c>
-      <c r="D38" t="n">
-        <v>81</v>
-      </c>
-      <c r="E38" t="inlineStr">
-        <is>
-          <t>0xe001</t>
-        </is>
-      </c>
-      <c r="F38" t="inlineStr">
-        <is>
-          <t>0x0e00</t>
-        </is>
-      </c>
-      <c r="G38" t="inlineStr">
-        <is>
-          <t>0x02:0xFD:0x80:0x01:0x00:0x00:0x00:0x07:0xE0:0x01:0x0E:0x00:0x7F:0x27:0x22</t>
-        </is>
-      </c>
-      <c r="H38" t="inlineStr">
-        <is>
-          <t>0x7F:0x27:0x22</t>
+          <t>0x3F</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>0x01</t>
         </is>
       </c>
     </row>

</xml_diff>